<commit_message>
Tarefas 1.1 + 1.2
</commit_message>
<xml_diff>
--- a/Trabalho2/Dados Habitantes 1940-2021.xlsx
+++ b/Trabalho2/Dados Habitantes 1940-2021.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uabpt-my.sharepoint.com/personal/1103691_estudante_uab_pt/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grupo EMAC\OneDrive - Universidade Aberta\Documents\GitHub\Visualiza-o-de-Informa-o-2025-26\Trabalho2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="32" documentId="8_{50E86F54-D770-42D7-A5CF-47BD6AA07B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BCC7CEDC-7042-4217-B6F9-0F61D0BE878C}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D747F6-56B9-4E99-9B51-783B3274C3DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FC2C6020-DB08-4479-BF17-FEDF7095C0C3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FC2C6020-DB08-4479-BF17-FEDF7095C0C3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Dados Consolidados Habitantes" sheetId="1" r:id="rId1"/>
+    <sheet name="Habitantes" sheetId="1" r:id="rId1"/>
+    <sheet name="1970" sheetId="3" r:id="rId2"/>
+    <sheet name="Referencias" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -44,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>Aveiro</t>
   </si>
@@ -146,6 +148,9 @@
   </si>
   <si>
     <t>UL - 2001 - 2021</t>
+  </si>
+  <si>
+    <t>Removido 1970 pela questão das habitações</t>
   </si>
 </sst>
 </file>
@@ -289,7 +294,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{79A96E9D-FD04-4AD5-ACF6-BD0D9B21D509}"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="9">
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
@@ -301,32 +306,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFF9F9F9"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -549,14 +528,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73B2320E-5643-4720-9962-94734675691E}" name="Tabela3" displayName="Tabela3" ref="A1:J21" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="A1:J21" xr:uid="{73B2320E-5643-4720-9962-94734675691E}"/>
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{282FBB24-FEE9-4A6E-AD22-5F7E451912B7}" name="Distrito" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{04A3E1D2-4C09-4842-88DA-DE930C25FE70}" name="1940" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{EB735F8B-B043-40CB-BD03-4BF5A553C0E5}" name="1950" dataDxfId="5"/>
-    <tableColumn id="4" xr3:uid="{C0983DD8-D6B3-40BE-AD8C-EEC1899624DF}" name="1960" dataDxfId="4"/>
-    <tableColumn id="5" xr3:uid="{5F315D01-F7C1-45C9-A3FC-C12F293E2659}" name="1970" dataDxfId="3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{73B2320E-5643-4720-9962-94734675691E}" name="Tabela3" displayName="Tabela3" ref="A1:I21" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="A1:I21" xr:uid="{73B2320E-5643-4720-9962-94734675691E}"/>
+  <tableColumns count="9">
+    <tableColumn id="1" xr3:uid="{282FBB24-FEE9-4A6E-AD22-5F7E451912B7}" name="Distrito" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{04A3E1D2-4C09-4842-88DA-DE930C25FE70}" name="1940" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{EB735F8B-B043-40CB-BD03-4BF5A553C0E5}" name="1950" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{C0983DD8-D6B3-40BE-AD8C-EEC1899624DF}" name="1960" dataDxfId="3"/>
     <tableColumn id="6" xr3:uid="{6384F49D-4F29-4F52-886F-828A2366739F}" name="1981" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{93D20A11-2117-4E87-B097-77CAFE75AE01}" name="1991" dataDxfId="1"/>
     <tableColumn id="8" xr3:uid="{B102EFD7-B5D6-4FC1-95C6-E59CC5994573}" name="2001"/>
@@ -884,18 +862,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3056D66-0D73-4C08-A58C-C65B8A23B6B4}">
-  <dimension ref="A1:J28"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="12.85546875" customWidth="1"/>
+    <col min="1" max="6" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>18</v>
       </c>
@@ -909,25 +887,22 @@
         <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="F1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -941,25 +916,22 @@
         <v>522227</v>
       </c>
       <c r="E2" s="3">
-        <v>539688</v>
+        <v>619966</v>
       </c>
       <c r="F2" s="3">
-        <v>619966</v>
+        <v>654265</v>
       </c>
       <c r="G2" s="3">
-        <v>654265</v>
+        <v>715142</v>
       </c>
       <c r="H2" s="3">
-        <v>715142</v>
-      </c>
-      <c r="I2" s="3">
         <v>714896</v>
       </c>
-      <c r="J2" s="4">
+      <c r="I2" s="4">
         <v>708902</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
@@ -973,25 +945,22 @@
         <v>268911</v>
       </c>
       <c r="E3">
-        <v>201502</v>
+        <v>184252</v>
       </c>
       <c r="F3">
-        <v>184252</v>
+        <v>169438</v>
       </c>
       <c r="G3">
-        <v>169438</v>
+        <v>160803</v>
       </c>
       <c r="H3">
-        <v>160803</v>
-      </c>
-      <c r="I3">
         <v>152170</v>
       </c>
-      <c r="J3" s="6">
+      <c r="I3" s="6">
         <v>146353</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
@@ -1005,25 +974,22 @@
         <v>593587</v>
       </c>
       <c r="E4">
-        <v>607354</v>
+        <v>709763</v>
       </c>
       <c r="F4">
-        <v>709763</v>
+        <v>748192</v>
       </c>
       <c r="G4">
-        <v>748192</v>
+        <v>835186</v>
       </c>
       <c r="H4">
-        <v>835186</v>
-      </c>
-      <c r="I4">
         <v>848861</v>
       </c>
-      <c r="J4" s="6">
+      <c r="I4" s="6">
         <v>850128</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
@@ -1037,25 +1003,22 @@
         <v>230266</v>
       </c>
       <c r="E5">
-        <v>176246</v>
+        <v>181375</v>
       </c>
       <c r="F5">
-        <v>181375</v>
+        <v>157809</v>
       </c>
       <c r="G5">
-        <v>157809</v>
+        <v>148163</v>
       </c>
       <c r="H5">
-        <v>148163</v>
-      </c>
-      <c r="I5">
         <v>134780</v>
       </c>
-      <c r="J5" s="6">
+      <c r="I5" s="6">
         <v>122452</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
@@ -1069,25 +1032,22 @@
         <v>310745</v>
       </c>
       <c r="E6">
-        <v>250351</v>
+        <v>232967</v>
       </c>
       <c r="F6">
-        <v>232967</v>
+        <v>214853</v>
       </c>
       <c r="G6">
-        <v>214853</v>
+        <v>207485</v>
       </c>
       <c r="H6">
-        <v>207485</v>
-      </c>
-      <c r="I6">
         <v>194541</v>
       </c>
-      <c r="J6" s="6">
+      <c r="I6" s="6">
         <v>178664</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -1101,25 +1061,22 @@
         <v>433596</v>
       </c>
       <c r="E7">
-        <v>398678</v>
+        <v>441001</v>
       </c>
       <c r="F7">
-        <v>441001</v>
+        <v>427839</v>
       </c>
       <c r="G7">
-        <v>427839</v>
+        <v>441034</v>
       </c>
       <c r="H7">
-        <v>441034</v>
-      </c>
-      <c r="I7">
         <v>430261</v>
       </c>
-      <c r="J7" s="6">
+      <c r="I7" s="6">
         <v>411510</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -1133,25 +1090,22 @@
         <v>215186</v>
       </c>
       <c r="E8">
-        <v>175286</v>
+        <v>179241</v>
       </c>
       <c r="F8">
-        <v>179241</v>
+        <v>173654</v>
       </c>
       <c r="G8">
-        <v>173654</v>
+        <v>173400</v>
       </c>
       <c r="H8">
-        <v>173400</v>
-      </c>
-      <c r="I8">
         <v>165766</v>
       </c>
-      <c r="J8" s="6">
+      <c r="I8" s="6">
         <v>153507</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
@@ -1165,25 +1119,22 @@
         <v>312509</v>
       </c>
       <c r="E9">
-        <v>265225</v>
+        <v>328605</v>
       </c>
       <c r="F9">
-        <v>328605</v>
+        <v>341404</v>
       </c>
       <c r="G9">
-        <v>341404</v>
+        <v>400937</v>
       </c>
       <c r="H9">
-        <v>400937</v>
-      </c>
-      <c r="I9">
         <v>452321</v>
       </c>
-      <c r="J9" s="6">
+      <c r="I9" s="6">
         <v>469983</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>8</v>
       </c>
@@ -1197,25 +1148,22 @@
         <v>276470</v>
       </c>
       <c r="E10">
-        <v>207469</v>
+        <v>205405</v>
       </c>
       <c r="F10">
-        <v>205405</v>
+        <v>188165</v>
       </c>
       <c r="G10">
-        <v>188165</v>
+        <v>178789</v>
       </c>
       <c r="H10">
-        <v>178789</v>
-      </c>
-      <c r="I10">
         <v>161144</v>
       </c>
-      <c r="J10" s="6">
+      <c r="I10" s="6">
         <v>142868</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
@@ -1229,25 +1177,22 @@
         <v>400275</v>
       </c>
       <c r="E11">
-        <v>374535</v>
+        <v>418942</v>
       </c>
       <c r="F11">
-        <v>418942</v>
+        <v>426152</v>
       </c>
       <c r="G11">
-        <v>426152</v>
+        <v>461605</v>
       </c>
       <c r="H11">
-        <v>461605</v>
-      </c>
-      <c r="I11">
         <v>472053</v>
       </c>
-      <c r="J11" s="6">
+      <c r="I11" s="6">
         <v>465169</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>10</v>
       </c>
@@ -1261,25 +1206,22 @@
         <v>1402586</v>
       </c>
       <c r="E12">
-        <v>1578614</v>
+        <v>2085861</v>
       </c>
       <c r="F12">
-        <v>2085861</v>
+        <v>2048180</v>
       </c>
       <c r="G12">
-        <v>2048180</v>
+        <v>2148125</v>
       </c>
       <c r="H12">
-        <v>2148125</v>
-      </c>
-      <c r="I12">
         <v>2245962</v>
       </c>
-      <c r="J12" s="6">
+      <c r="I12" s="6">
         <v>2287869</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>11</v>
       </c>
@@ -1293,25 +1235,22 @@
         <v>183841</v>
       </c>
       <c r="E13">
-        <v>143903</v>
+        <v>142141</v>
       </c>
       <c r="F13">
-        <v>142141</v>
+        <v>134169</v>
       </c>
       <c r="G13">
-        <v>134169</v>
+        <v>126549</v>
       </c>
       <c r="H13">
-        <v>126549</v>
-      </c>
-      <c r="I13">
         <v>118201</v>
       </c>
-      <c r="J13" s="6">
+      <c r="I13" s="6">
         <v>105031</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>12</v>
       </c>
@@ -1325,25 +1264,22 @@
         <v>1191504</v>
       </c>
       <c r="E14">
-        <v>1302786</v>
+        <v>1561310</v>
       </c>
       <c r="F14">
-        <v>1561310</v>
+        <v>1641501</v>
       </c>
       <c r="G14">
-        <v>1641501</v>
+        <v>1788658</v>
       </c>
       <c r="H14">
-        <v>1788658</v>
-      </c>
-      <c r="I14">
         <v>1817425</v>
       </c>
-      <c r="J14" s="6">
+      <c r="I14" s="6">
         <v>1803223</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>13</v>
       </c>
@@ -1357,25 +1293,22 @@
         <v>462121</v>
       </c>
       <c r="E15">
-        <v>427892</v>
+        <v>458229</v>
       </c>
       <c r="F15">
-        <v>458229</v>
+        <v>444880</v>
       </c>
       <c r="G15">
-        <v>444880</v>
+        <v>455374</v>
       </c>
       <c r="H15">
-        <v>455374</v>
-      </c>
-      <c r="I15">
         <v>453429</v>
       </c>
-      <c r="J15" s="6">
+      <c r="I15" s="6">
         <v>431633</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="5" t="s">
         <v>14</v>
       </c>
@@ -1389,25 +1322,22 @@
         <v>376128</v>
       </c>
       <c r="E16">
-        <v>465367</v>
+        <v>654312</v>
       </c>
       <c r="F16">
-        <v>654312</v>
+        <v>712594</v>
       </c>
       <c r="G16">
-        <v>712594</v>
+        <v>795222</v>
       </c>
       <c r="H16">
-        <v>795222</v>
-      </c>
-      <c r="I16">
         <v>858940</v>
       </c>
-      <c r="J16" s="6">
+      <c r="I16" s="6">
         <v>882588</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="5" t="s">
         <v>15</v>
       </c>
@@ -1421,25 +1351,22 @@
         <v>275345</v>
       </c>
       <c r="E17">
-        <v>249919</v>
+        <v>255395</v>
       </c>
       <c r="F17">
-        <v>255395</v>
+        <v>250059</v>
       </c>
       <c r="G17">
-        <v>250059</v>
+        <v>250491</v>
       </c>
       <c r="H17">
-        <v>250491</v>
-      </c>
-      <c r="I17">
         <v>243380</v>
       </c>
-      <c r="J17" s="6">
+      <c r="I17" s="6">
         <v>231882</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="5" t="s">
         <v>16</v>
       </c>
@@ -1453,25 +1380,22 @@
         <v>322649</v>
       </c>
       <c r="E18">
-        <v>261995</v>
+        <v>263972</v>
       </c>
       <c r="F18">
-        <v>263972</v>
+        <v>236294</v>
       </c>
       <c r="G18">
-        <v>236294</v>
+        <v>222781</v>
       </c>
       <c r="H18">
-        <v>222781</v>
-      </c>
-      <c r="I18">
         <v>204474</v>
       </c>
-      <c r="J18" s="6">
+      <c r="I18" s="6">
         <v>185148</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="5" t="s">
         <v>17</v>
       </c>
@@ -1485,25 +1409,22 @@
         <v>477468</v>
       </c>
       <c r="E19">
-        <v>407538</v>
+        <v>421752</v>
       </c>
       <c r="F19">
-        <v>421752</v>
+        <v>401871</v>
       </c>
       <c r="G19">
-        <v>401871</v>
+        <v>394369</v>
       </c>
       <c r="H19">
-        <v>394369</v>
-      </c>
-      <c r="I19">
         <v>375857</v>
       </c>
-      <c r="J19" s="6">
+      <c r="I19" s="6">
         <v>352720</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>19</v>
       </c>
@@ -1517,25 +1438,22 @@
         <v>327806</v>
       </c>
       <c r="E20">
-        <v>284161</v>
+        <v>249101</v>
       </c>
       <c r="F20">
-        <v>249101</v>
+        <v>237795</v>
       </c>
       <c r="G20">
-        <v>237795</v>
+        <v>242544</v>
       </c>
       <c r="H20">
-        <v>242544</v>
-      </c>
-      <c r="I20">
         <v>247095</v>
       </c>
-      <c r="J20" s="6">
+      <c r="I20" s="6">
         <v>238794</v>
       </c>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
@@ -1549,45 +1467,19 @@
         <v>268069</v>
       </c>
       <c r="E21" s="8">
-        <v>250174</v>
+        <v>259251</v>
       </c>
       <c r="F21" s="8">
-        <v>259251</v>
+        <v>253425</v>
       </c>
       <c r="G21" s="8">
-        <v>253425</v>
+        <v>248012</v>
       </c>
       <c r="H21" s="8">
-        <v>248012</v>
-      </c>
-      <c r="I21" s="8">
         <v>279336</v>
       </c>
-      <c r="J21" s="9">
+      <c r="I21" s="9">
         <v>252693</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1596,6 +1488,172 @@
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D424077-B588-4F35-9169-B5F3EF21793F}">
+  <dimension ref="A1:A24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
+        <v>539688</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>201502</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>607354</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>176246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>250351</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>398678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>175286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>265225</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>207469</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>374535</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>1578614</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>143903</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>1302786</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>427892</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>465367</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>249919</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>261995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>407538</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>284161</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="8">
+        <v>250174</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF4D013F-071F-4DCC-80F2-F7FB832561A7}">
+  <dimension ref="A1:A6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1"/>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>